<commit_message>
update generator + template
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP021_F1.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP021_F1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22920" windowHeight="5640"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22920" windowHeight="4785"/>
   </bookViews>
   <sheets>
     <sheet name="A4縦2人" sheetId="3" r:id="rId1"/>
@@ -82,7 +82,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,13 +149,28 @@
       <family val="1"/>
       <charset val="128"/>
     </font>
+    <font>
+      <u val="double"/>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="IPA明朝"/>
+      <family val="1"/>
+      <charset val="128"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -228,7 +243,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -239,12 +254,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -268,23 +277,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -588,7 +606,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -599,7 +617,7 @@
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="9.75" customHeight="1"/>
@@ -609,26 +627,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="9.75" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="15" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
       <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:19" ht="9.75" customHeight="1">
@@ -640,79 +658,79 @@
         <v>4</v>
       </c>
       <c r="D2" s="13"/>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
     </row>
     <row r="3" spans="1:19" ht="9.75" customHeight="1">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="17" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:19" ht="9.75" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:19" ht="9.75" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="5"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="17"/>
     </row>
     <row r="6" spans="1:19" ht="9.75" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -731,11 +749,13 @@
       <c r="S6" s="3"/>
     </row>
     <row r="11" spans="1:19" ht="9.75" customHeight="1">
-      <c r="M11" s="6"/>
-      <c r="N11" s="7"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I1:L2"/>
+    <mergeCell ref="I3:L3"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="A1:B1"/>
@@ -744,8 +764,6 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
-    <mergeCell ref="I1:L2"/>
-    <mergeCell ref="I3:L3"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>